<commit_message>
finish to add basic functions
</commit_message>
<xml_diff>
--- a/src/main_DB.xlsx
+++ b/src/main_DB.xlsx
@@ -670,7 +670,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" outlineLevelCol="0"/>
   <cols>
     <col width="12" customWidth="1" style="13" min="2" max="2"/>
     <col width="14" customWidth="1" style="13" min="3" max="3"/>
@@ -724,7 +724,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="20"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="20" outlineLevelCol="0"/>
   <cols>
     <col width="20.7109375" customWidth="1" style="13" min="1" max="1"/>
     <col width="22.7109375" customWidth="1" style="13" min="2" max="2"/>
@@ -2470,7 +2470,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="20"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="20" outlineLevelCol="0"/>
   <cols>
     <col width="49.42578125" customWidth="1" style="13" min="2" max="2"/>
     <col width="25" customWidth="1" style="13" min="3" max="3"/>
@@ -17585,7 +17585,7 @@
       <selection activeCell="I985" sqref="I985"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="20"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="20" outlineLevelCol="0"/>
   <cols>
     <col width="16.42578125" customWidth="1" style="13" min="2" max="2"/>
     <col width="17.85546875" customWidth="1" style="13" min="4" max="4"/>

</xml_diff>